<commit_message>
mise a jour du fichier excel gantt
</commit_message>
<xml_diff>
--- a/project/gestion_projet_e2/diagramme_gantt_projet_e2.xlsx
+++ b/project/gestion_projet_e2/diagramme_gantt_projet_e2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr dateCompatibility="0" filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C691CF39-7EDA-4552-99A5-D073D8B01D97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B42C73BD-99A9-4356-A930-028E9B674330}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="415" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -659,7 +659,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="61">
+  <fills count="62">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1005,6 +1005,12 @@
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor rgb="FFC8F0FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -2046,32 +2052,32 @@
     <xf numFmtId="0" fontId="14" fillId="56" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="3" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="61" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="61" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="61" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="16" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="9" fontId="16" fillId="61" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1">
+    <xf numFmtId="14" fontId="0" fillId="61" borderId="0" xfId="9" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="49" fillId="2" borderId="0" xfId="10" applyFont="1" applyFill="1">
+    <xf numFmtId="165" fontId="49" fillId="61" borderId="0" xfId="10" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="10" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="61" borderId="0" xfId="10" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="61" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="61" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="61" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3399,13 +3405,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="31745" name="Barre de défilement 1" descr="Défiler la barre pour faire défiler la chronologie du projet Gantt.">
+        <xdr:cNvPr id="32769" name="Barre de défilement 1" descr="Défiler la barre pour faire défiler la chronologie du projet Gantt.">
           <a:extLst>
             <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
               <a14:compatExt xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" spid="_x0000_s16385"/>
             </a:ext>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A9CEFFA-3EA1-4C47-AF20-B99DA49052D2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4496D7DD-699F-4798-8CB1-8914B5266955}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3462,13 +3468,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="32769" name="Barre de défilement 1" descr="Défiler la barre pour faire défiler la chronologie du projet Gantt.">
+        <xdr:cNvPr id="33793" name="Barre de défilement 1" descr="Défiler la barre pour faire défiler la chronologie du projet Gantt.">
           <a:extLst>
             <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
               <a14:compatExt xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" spid="_x0000_s13313"/>
             </a:ext>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{044CAB63-8507-44B4-A523-950FD419C369}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F388E95-E4C7-4EC7-B422-55C9CE4B00C1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3525,13 +3531,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="33793" name="Barre de défilement 1" descr="Défiler la barre pour faire défiler la chronologie du projet Gantt.">
+        <xdr:cNvPr id="34817" name="Barre de défilement 1" descr="Défiler la barre pour faire défiler la chronologie du projet Gantt.">
           <a:extLst>
             <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
               <a14:compatExt xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" spid="_x0000_s17409"/>
             </a:ext>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90669D78-D9E6-4042-B1B5-D677D9E48AFB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BEDF6A9-500C-409B-984C-5897E7A2E887}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11363,7 +11369,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <controls>
-    <control shapeId="31745" r:id="rId4" name="Barre de défilement 1">
+    <control shapeId="32769" r:id="rId4" name="Barre de défilement 1">
       <controlPr defaultSize="0" autoPict="0" altText="Défiler la barre pour faire défiler la chronologie du projet Gantt.">
         <anchor moveWithCells="1">
           <from>
@@ -18727,7 +18733,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <controls>
-    <control shapeId="32769" r:id="rId4" name="Barre de défilement 1">
+    <control shapeId="33793" r:id="rId4" name="Barre de défilement 1">
       <controlPr defaultSize="0" autoPict="0" altText="Défiler la barre pour faire défiler la chronologie du projet Gantt.">
         <anchor moveWithCells="1">
           <from>
@@ -18819,7 +18825,7 @@
   <dimension ref="A1:BR142"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -27837,7 +27843,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <controls>
-    <control shapeId="33793" r:id="rId4" name="Barre de défilement 1">
+    <control shapeId="34817" r:id="rId4" name="Barre de défilement 1">
       <controlPr defaultSize="0" autoPict="0" altText="Défiler la barre pour faire défiler la chronologie du projet Gantt.">
         <anchor moveWithCells="1">
           <from>
@@ -28092,6 +28098,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="22a266b9fa9a230c5a512669d8b298c3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eddc33fff6b14141ee5c74a0d29ea6a1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -28367,15 +28382,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://purl.oclc.org/ooxml/officeDocument/customXml" ds:itemID="{AA4BA2A8-DB97-40F9-8DB6-154C09C7467C}">
   <ds:schemaRefs>
@@ -28389,6 +28395,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://purl.oclc.org/ooxml/officeDocument/customXml" ds:itemID="{39060724-9CA2-4290-8A0C-B53624A594E7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://purl.oclc.org/ooxml/officeDocument/customXml" ds:itemID="{75C87518-DD8E-42CD-8DAC-291A323E849B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -28407,12 +28421,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://purl.oclc.org/ooxml/officeDocument/customXml" ds:itemID="{39060724-9CA2-4290-8A0C-B53624A594E7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>